<commit_message>
primer resultado orsh. gasto todo mal
</commit_message>
<xml_diff>
--- a/poverty_measurement/input/canastapercapita_metocchi_sin_outliars.xlsx
+++ b/poverty_measurement/input/canastapercapita_metocchi_sin_outliars.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>bien</t>
   </si>
@@ -48,12 +48,12 @@
     <t>Lentejas</t>
   </si>
   <si>
+    <t>Margarina/Mantequilla</t>
+  </si>
+  <si>
     <t>Cambur</t>
   </si>
   <si>
-    <t>Margarina/Mantequilla</t>
-  </si>
-  <si>
     <t>Carne de pollo</t>
   </si>
   <si>
@@ -69,10 +69,13 @@
     <t>Leche en polvo, completa o descremada</t>
   </si>
   <si>
+    <t>Caraotas</t>
+  </si>
+  <si>
     <t>Pescado fresco</t>
   </si>
   <si>
-    <t>Caraotas</t>
+    <t>Hueso de res, pata de res, pata de pollo</t>
   </si>
   <si>
     <t>Papas</t>
@@ -157,7 +160,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -165,19 +168,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2">
@@ -185,19 +188,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>96.784046447030207</v>
+        <v>95.84398269395831</v>
       </c>
       <c r="C2" s="1">
-        <v>120.40946841446973</v>
+        <v>117.98951321053738</v>
       </c>
       <c r="D2" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E2" s="1">
         <v>383</v>
       </c>
       <c r="F2" s="1">
-        <v>461.16827392578125</v>
+        <v>451.89984130859375</v>
       </c>
     </row>
     <row r="3">
@@ -205,19 +208,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>88.178740510322612</v>
+        <v>88.527556184735843</v>
       </c>
       <c r="C3" s="1">
-        <v>109.70356874204749</v>
+        <v>108.98256720942982</v>
       </c>
       <c r="D3" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E3" s="1">
         <v>345</v>
       </c>
       <c r="F3" s="1">
-        <v>378.47732543945313</v>
+        <v>375.9898681640625</v>
       </c>
     </row>
     <row r="4">
@@ -225,19 +228,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>20.414505508834708</v>
+        <v>20.572643868753406</v>
       </c>
       <c r="C4" s="1">
-        <v>25.397778099329376</v>
+        <v>25.326121149435664</v>
       </c>
       <c r="D4" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E4" s="1">
         <v>900</v>
       </c>
       <c r="F4" s="1">
-        <v>228.58000183105469</v>
+        <v>227.93508911132813</v>
       </c>
     </row>
     <row r="5">
@@ -245,19 +248,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>29.721348327402282</v>
+        <v>29.627309096088855</v>
       </c>
       <c r="C5" s="1">
-        <v>36.976462853456546</v>
+        <v>36.472938917393705</v>
       </c>
       <c r="D5" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E5" s="1">
         <v>393.5</v>
       </c>
       <c r="F5" s="1">
-        <v>145.50238037109375</v>
+        <v>143.52101135253906</v>
       </c>
     </row>
     <row r="6">
@@ -265,19 +268,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>20.197538508043817</v>
+        <v>20.343764140321884</v>
       </c>
       <c r="C6" s="1">
-        <v>25.127848309202836</v>
+        <v>25.044355738134833</v>
       </c>
       <c r="D6" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E6" s="1">
         <v>368.5</v>
       </c>
       <c r="F6" s="1">
-        <v>92.596122741699219</v>
+        <v>92.2884521484375</v>
       </c>
     </row>
     <row r="7">
@@ -285,19 +288,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>35.766772508143426</v>
+        <v>36.502580301205612</v>
       </c>
       <c r="C7" s="1">
-        <v>44.497602806142275</v>
+        <v>44.936797849801273</v>
       </c>
       <c r="D7" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E7" s="1">
         <v>182.33332824707031</v>
       </c>
       <c r="F7" s="1">
-        <v>81.133956909179688</v>
+        <v>81.934761047363281</v>
       </c>
     </row>
     <row r="8">
@@ -305,19 +308,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>42.642428959061007</v>
+        <v>42.702860308868274</v>
       </c>
       <c r="C8" s="1">
-        <v>53.051637767391675</v>
+        <v>52.569702660840306</v>
       </c>
       <c r="D8" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E8" s="1">
         <v>137.5</v>
       </c>
       <c r="F8" s="1">
-        <v>72.945999145507813</v>
+        <v>72.283340454101563</v>
       </c>
     </row>
     <row r="9">
@@ -325,19 +328,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>29.041417000527851</v>
+        <v>28.790801655308766</v>
       </c>
       <c r="C9" s="1">
-        <v>36.130557487069886</v>
+        <v>35.443149906535666</v>
       </c>
       <c r="D9" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E9" s="1">
         <v>196.5</v>
       </c>
       <c r="F9" s="1">
-        <v>70.996543884277344</v>
+        <v>69.645790100097656</v>
       </c>
     </row>
     <row r="10">
@@ -345,19 +348,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>13.350510630674496</v>
+        <v>13.490188612472839</v>
       </c>
       <c r="C10" s="1">
-        <v>16.609430331585003</v>
+        <v>16.607206108358476</v>
       </c>
       <c r="D10" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E10" s="1">
         <v>355</v>
       </c>
       <c r="F10" s="1">
-        <v>58.963478088378906</v>
+        <v>58.955581665039063</v>
       </c>
     </row>
     <row r="11">
@@ -365,19 +368,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>16.592709721289403</v>
+        <v>16.901307093787345</v>
       </c>
       <c r="C11" s="1">
-        <v>20.643064700848434</v>
+        <v>20.806491048441437</v>
       </c>
       <c r="D11" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E11" s="1">
         <v>254.5</v>
       </c>
       <c r="F11" s="1">
-        <v>52.536598205566406</v>
+        <v>52.952518463134766</v>
       </c>
     </row>
     <row r="12">
@@ -385,19 +388,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>30.442743446640595</v>
+        <v>5.8410878431704489</v>
       </c>
       <c r="C12" s="1">
-        <v>37.873954114232291</v>
+        <v>7.1907184984971249</v>
       </c>
       <c r="D12" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E12" s="1">
-        <v>113.375</v>
+        <v>584</v>
       </c>
       <c r="F12" s="1">
-        <v>42.939594268798828</v>
+        <v>41.993797302246094</v>
       </c>
     </row>
     <row r="13">
@@ -405,19 +408,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>5.8559978520304821</v>
+        <v>29.979799272561049</v>
       </c>
       <c r="C13" s="1">
-        <v>7.2854731993111432</v>
+        <v>36.906875161033526</v>
       </c>
       <c r="D13" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E13" s="1">
-        <v>584</v>
+        <v>113.375</v>
       </c>
       <c r="F13" s="1">
-        <v>42.547164916992188</v>
+        <v>41.843170166015625</v>
       </c>
     </row>
     <row r="14">
@@ -425,19 +428,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>17.96927238561825</v>
+        <v>17.472639226929545</v>
       </c>
       <c r="C14" s="1">
-        <v>22.355652523423007</v>
+        <v>21.509834220672516</v>
       </c>
       <c r="D14" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E14" s="1">
         <v>174</v>
       </c>
       <c r="F14" s="1">
-        <v>38.898834228515625</v>
+        <v>37.427112579345703</v>
       </c>
     </row>
     <row r="15">
@@ -445,19 +448,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>17.062219975865833</v>
+        <v>17.108143586948277</v>
       </c>
       <c r="C15" s="1">
-        <v>21.227184595708138</v>
+        <v>21.061118991721774</v>
       </c>
       <c r="D15" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E15" s="1">
         <v>164.85714721679688</v>
       </c>
       <c r="F15" s="1">
-        <v>34.994529724121094</v>
+        <v>34.720760345458984</v>
       </c>
     </row>
     <row r="16">
@@ -465,19 +468,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>6.7396700205449349</v>
+        <v>6.496793987378453</v>
       </c>
       <c r="C16" s="1">
-        <v>8.384853728070766</v>
+        <v>7.9979308518130674</v>
       </c>
       <c r="D16" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E16" s="1">
         <v>405.84616088867188</v>
       </c>
       <c r="F16" s="1">
-        <v>34.029605865478516</v>
+        <v>32.459297180175781</v>
       </c>
     </row>
     <row r="17">
@@ -485,19 +488,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>16.993987975951903</v>
+        <v>17.348970637867026</v>
       </c>
       <c r="C17" s="1">
-        <v>21.142297561278564</v>
+        <v>21.357590597785489</v>
       </c>
       <c r="D17" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E17" s="1">
         <v>145</v>
       </c>
       <c r="F17" s="1">
-        <v>30.656332015991211</v>
+        <v>30.968505859375</v>
       </c>
     </row>
     <row r="18">
@@ -505,19 +508,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>5.4394504765948213</v>
+        <v>5.428860857967102</v>
       </c>
       <c r="C18" s="1">
-        <v>6.7672447183566966</v>
+        <v>6.6832431293684529</v>
       </c>
       <c r="D18" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E18" s="1">
         <v>428.5</v>
       </c>
       <c r="F18" s="1">
-        <v>28.997644424438477</v>
+        <v>28.637697219848633</v>
       </c>
     </row>
     <row r="19">
@@ -525,19 +528,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>27.056494602618731</v>
+        <v>16.219083439044521</v>
       </c>
       <c r="C19" s="1">
-        <v>33.661106759417272</v>
+        <v>19.966634064802157</v>
       </c>
       <c r="D19" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E19" s="1">
-        <v>85</v>
+        <v>135.11111450195313</v>
       </c>
       <c r="F19" s="1">
-        <v>28.611940383911133</v>
+        <v>26.977142333984375</v>
       </c>
     </row>
     <row r="20">
@@ -545,19 +548,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>16.34698014077777</v>
+        <v>25.531556500561368</v>
       </c>
       <c r="C20" s="1">
-        <v>20.337351352434279</v>
+        <v>31.430829844119135</v>
       </c>
       <c r="D20" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E20" s="1">
-        <v>135.11111450195313</v>
+        <v>85</v>
       </c>
       <c r="F20" s="1">
-        <v>27.478021621704102</v>
+        <v>26.716205596923828</v>
       </c>
     </row>
     <row r="21">
@@ -565,19 +568,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>14.884531398255904</v>
+        <v>10.323031969743123</v>
       </c>
       <c r="C21" s="1">
-        <v>18.517912365869435</v>
+        <v>12.708252231534816</v>
       </c>
       <c r="D21" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E21" s="1">
-        <v>122.46154022216797</v>
+        <v>183.25</v>
       </c>
       <c r="F21" s="1">
-        <v>22.67732048034668</v>
+        <v>23.287872314453125</v>
       </c>
     </row>
     <row r="22">
@@ -585,19 +588,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>13.255558987339098</v>
+        <v>14.784726334712492</v>
       </c>
       <c r="C22" s="1">
-        <v>16.491300379027503</v>
+        <v>18.200857185005859</v>
       </c>
       <c r="D22" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E22" s="1">
-        <v>40</v>
+        <v>122.46154022216797</v>
       </c>
       <c r="F22" s="1">
-        <v>6.596519947052002</v>
+        <v>22.28904914855957</v>
       </c>
     </row>
     <row r="23">
@@ -605,19 +608,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>1.7076057000564748</v>
+        <v>13.48392100532112</v>
       </c>
       <c r="C23" s="1">
-        <v>2.124439910641494</v>
+        <v>16.59949027578693</v>
       </c>
       <c r="D23" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E23" s="1">
-        <v>284.66665649414063</v>
+        <v>40</v>
       </c>
       <c r="F23" s="1">
-        <v>6.047572135925293</v>
+        <v>6.639796257019043</v>
       </c>
     </row>
     <row r="24">
@@ -625,19 +628,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>7.0741484504424497</v>
+        <v>1.6589364201645171</v>
       </c>
       <c r="C24" s="1">
-        <v>8.8009797912003922</v>
+        <v>2.0422471421737747</v>
       </c>
       <c r="D24" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E24" s="1">
-        <v>56.5</v>
+        <v>284.66665649414063</v>
       </c>
       <c r="F24" s="1">
-        <v>4.9725537300109863</v>
+        <v>5.8135967254638672</v>
       </c>
     </row>
     <row r="25">
@@ -645,19 +648,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>10.161943102488138</v>
+        <v>7.0618583100332106</v>
       </c>
       <c r="C25" s="1">
-        <v>12.642519080169055</v>
+        <v>8.693557914993951</v>
       </c>
       <c r="D25" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E25" s="1">
-        <v>35</v>
+        <v>56.5</v>
       </c>
       <c r="F25" s="1">
-        <v>4.4248814582824707</v>
+        <v>4.9118599891662598</v>
       </c>
     </row>
     <row r="26">
@@ -665,19 +668,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>8.9211758812348201</v>
+        <v>10.661347274316794</v>
       </c>
       <c r="C26" s="1">
-        <v>11.098874936202565</v>
+        <v>13.124738045813785</v>
       </c>
       <c r="D26" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E26" s="1">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F26" s="1">
-        <v>2.5527412891387939</v>
+        <v>4.593658447265625</v>
       </c>
     </row>
     <row r="27">
@@ -685,19 +688,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>10.834526434212266</v>
+        <v>9.3319514191235147</v>
       </c>
       <c r="C27" s="1">
-        <v>13.479282872232503</v>
+        <v>11.488174438154701</v>
       </c>
       <c r="D27" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E27" s="1">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="F27" s="1">
-        <v>0.67396414279937744</v>
+        <v>2.642280101776123</v>
       </c>
     </row>
     <row r="28">
@@ -705,18 +708,38 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>17.856761607752695</v>
+        <v>10.916542360439037</v>
       </c>
       <c r="C28" s="1">
-        <v>22.215677148036026</v>
+        <v>13.438897903087048</v>
       </c>
       <c r="D28" s="1">
-        <v>2994</v>
+        <v>2963</v>
       </c>
       <c r="E28" s="1">
+        <v>5</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.67194491624832153</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1">
+        <v>18.153271772593531</v>
+      </c>
+      <c r="C29" s="1">
+        <v>22.347732282272272</v>
+      </c>
+      <c r="D29" s="1">
+        <v>2963</v>
+      </c>
+      <c r="E29" s="1">
         <v>0</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F29" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>